<commit_message>
Ready to do code naive bayes test 2
</commit_message>
<xml_diff>
--- a/Code/Scratchpad/NBayes1ExploratoryResults.xlsx
+++ b/Code/Scratchpad/NBayes1ExploratoryResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacqu\city\DS2020\Modules\MachineLearning\CourseworkWip\Code\Scratchpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211AD17F-37DA-49A3-B307-E1A86CBA8F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A56E30-83B8-49C0-BD6E-F7D392353F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25980" yWindow="300" windowWidth="12315" windowHeight="11775" xr2:uid="{ECAA2E89-BD46-444A-94F2-3166C2423E19}"/>
+    <workbookView xWindow="3270" yWindow="2730" windowWidth="16245" windowHeight="11835" xr2:uid="{ECAA2E89-BD46-444A-94F2-3166C2423E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
   <si>
     <t>Distribution Tpe</t>
   </si>
@@ -76,6 +76,10 @@
   </si>
   <si>
     <t>Optimized</t>
+  </si>
+  <si>
+    <t>Dataset
+Standardised?</t>
   </si>
 </sst>
 </file>
@@ -444,218 +448,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386772E0-3E24-4EF4-AD43-F70E16880A1D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="3" customWidth="1"/>
+    <col min="1" max="2" width="13.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
         <v>0.35</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.37</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5.92</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
         <v>0.23</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.25</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>7720.05</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.25900000000000001</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
         <v>0.35</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.37</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6.13</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
         <v>0.23</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.25</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7360.09</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.7277000000000001E-2</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
         <v>0.3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.32</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>601.64</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
         <v>0.23</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.25</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>7750.2</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.7277000000000001E-2</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8">
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
         <v>0.25</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.26</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>5185.5</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1.8402999999999999E-2</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0.31</v>
+      </c>
+      <c r="F9">
+        <v>0.32</v>
+      </c>
+      <c r="G9">
+        <v>385.67</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>0.25</v>
+      </c>
+      <c r="F10">
+        <v>0.26</v>
+      </c>
+      <c r="G10">
+        <v>4419.38</v>
+      </c>
+      <c r="H10">
+        <v>0.11377</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Looks like there might be line feed discrepancies when using git/github and 2 pc's
</commit_message>
<xml_diff>
--- a/Code/Scratchpad/NBayes1ExploratoryResults.xlsx
+++ b/Code/Scratchpad/NBayes1ExploratoryResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacqu\city\DS2020\Modules\MachineLearning\CourseworkWip\Code\Scratchpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A56E30-83B8-49C0-BD6E-F7D392353F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4FFDE8-84F6-4F3E-9567-A4E47EF92EDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="2730" windowWidth="16245" windowHeight="11835" xr2:uid="{ECAA2E89-BD46-444A-94F2-3166C2423E19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{ECAA2E89-BD46-444A-94F2-3166C2423E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>